<commit_message>
Added missing data preprocessing step and reorganized project structure
- Created a new notebook for data preprocessing to handle the missing preprocessing step.
- Added new directories ('product_datasets', 'pre_processed_datasets') for better project organization.
- Updated all notebooks to use relative data paths to ensure portability across machines.
</commit_message>
<xml_diff>
--- a/datasets/master_dataset/master_dataset.xlsx
+++ b/datasets/master_dataset/master_dataset.xlsx
@@ -1,63 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin\OneDrive\Documents\Infosys Springboard Internship Files\NitinMishra-Infosys-Nov24\datasets\master_dataset\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE74F49-FD96-4E0B-BBF4-70EC77617AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Day Index</t>
-  </si>
-  <si>
-    <t>Clicks</t>
-  </si>
-  <si>
-    <t>Impressions</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -72,44 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -397,2998 +424,3006 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Day Index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Clicks</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Impressions</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>44531</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>445</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>620</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>44532</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>433</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>890</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>44533</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>424</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>851</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>44534</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>427</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>881</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>44535</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>451</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>678</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>44536</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>429</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>995</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>44537</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>444</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>910</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>44538</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>431</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>867</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>44539</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>456</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>1128</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>44540</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>391</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>1129</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12">
+      <c r="A12" s="2" t="n">
         <v>44541</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>447</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>1461</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13">
+      <c r="A13" s="2" t="n">
         <v>44542</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>347</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>1237</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14">
+      <c r="A14" s="2" t="n">
         <v>44543</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>443</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>1403</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15">
+      <c r="A15" s="2" t="n">
         <v>44544</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>427</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>1641</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16">
+      <c r="A16" s="2" t="n">
         <v>44545</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>423</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>1496</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17">
+      <c r="A17" s="2" t="n">
         <v>44546</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>404</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>1775</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18">
+      <c r="A18" s="2" t="n">
         <v>44547</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>413</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>1619</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19">
+      <c r="A19" s="2" t="n">
         <v>44548</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>370</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="n">
         <v>969</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>44549</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>429</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>678</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>44550</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>383</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>1330</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22">
+      <c r="A22" s="2" t="n">
         <v>44551</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>379</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>1331</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23">
+      <c r="A23" s="2" t="n">
         <v>44552</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>350</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>1176</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24">
+      <c r="A24" s="2" t="n">
         <v>44553</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>359</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>1257</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25">
+      <c r="A25" s="2" t="n">
         <v>44554</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>339</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>1085</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26">
+      <c r="A26" s="2" t="n">
         <v>44555</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>338</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>1814</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27">
+      <c r="A27" s="2" t="n">
         <v>44556</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>398</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>1759</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>44557</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>369</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="n">
         <v>1119</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29">
+      <c r="A29" s="2" t="n">
         <v>44558</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>381</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>893</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30">
+      <c r="A30" s="2" t="n">
         <v>44559</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>361</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>1028</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31">
+      <c r="A31" s="2" t="n">
         <v>44560</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>356</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>956</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="32">
+      <c r="A32" s="2" t="n">
         <v>44561</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>237</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>911</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33">
+      <c r="A33" s="2" t="n">
         <v>44562</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>332</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>1350</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34">
+      <c r="A34" s="2" t="n">
         <v>44563</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>389</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>1704</v>
       </c>
-      <c r="D34">
+      <c r="D34" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35">
+      <c r="A35" s="2" t="n">
         <v>44564</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>411</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>2177</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="36">
+      <c r="A36" s="2" t="n">
         <v>44565</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>401</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>2549</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+    <row r="37">
+      <c r="A37" s="2" t="n">
         <v>44566</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>361</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>1915</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>44567</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>385</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>2125</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39">
+      <c r="A39" s="2" t="n">
         <v>44568</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="n">
         <v>397</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>1984</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+    <row r="40">
+      <c r="A40" s="2" t="n">
         <v>44569</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>398</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>1859</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="41">
+      <c r="A41" s="2" t="n">
         <v>44570</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="n">
         <v>401</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="n">
         <v>1759</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="42">
+      <c r="A42" s="2" t="n">
         <v>44571</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="n">
         <v>392</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="n">
         <v>1571</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43">
+      <c r="A43" s="2" t="n">
         <v>44572</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="n">
         <v>398</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="n">
         <v>1818</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="44">
+      <c r="A44" s="2" t="n">
         <v>44573</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="n">
         <v>376</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="n">
         <v>1506</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="45">
+      <c r="A45" s="2" t="n">
         <v>44574</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="n">
         <v>369</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="n">
         <v>1724</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46">
+      <c r="A46" s="2" t="n">
         <v>44575</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="n">
         <v>387</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="n">
         <v>2196</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="47">
+      <c r="A47" s="2" t="n">
         <v>44576</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="n">
         <v>399</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="n">
         <v>1933</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+    <row r="48">
+      <c r="A48" s="2" t="n">
         <v>44577</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="n">
         <v>413</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="n">
         <v>1959</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>44578</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="n">
         <v>425</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="n">
         <v>1689</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+    <row r="50">
+      <c r="A50" s="2" t="n">
         <v>44579</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="n">
         <v>368</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="n">
         <v>1524</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+    <row r="51">
+      <c r="A51" s="2" t="n">
         <v>44580</v>
       </c>
-      <c r="B51">
+      <c r="B51" t="n">
         <v>390</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="n">
         <v>1041</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+    <row r="52">
+      <c r="A52" s="2" t="n">
         <v>44581</v>
       </c>
-      <c r="B52">
+      <c r="B52" t="n">
         <v>431</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="n">
         <v>1175</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+    <row r="53">
+      <c r="A53" s="2" t="n">
         <v>44582</v>
       </c>
-      <c r="B53">
+      <c r="B53" t="n">
         <v>434</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="n">
         <v>1681</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+    <row r="54">
+      <c r="A54" s="2" t="n">
         <v>44583</v>
       </c>
-      <c r="B54">
+      <c r="B54" t="n">
         <v>385</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="n">
         <v>963</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+    <row r="55">
+      <c r="A55" s="2" t="n">
         <v>44584</v>
       </c>
-      <c r="B55">
+      <c r="B55" t="n">
         <v>444</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="n">
         <v>783</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+    <row r="56">
+      <c r="A56" s="2" t="n">
         <v>44585</v>
       </c>
-      <c r="B56">
+      <c r="B56" t="n">
         <v>425</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="n">
         <v>1040</v>
       </c>
-      <c r="D56">
+      <c r="D56" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+    <row r="57">
+      <c r="A57" s="2" t="n">
         <v>44586</v>
       </c>
-      <c r="B57">
+      <c r="B57" t="n">
         <v>384</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="n">
         <v>968</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+    <row r="58">
+      <c r="A58" s="2" t="n">
         <v>44587</v>
       </c>
-      <c r="B58">
+      <c r="B58" t="n">
         <v>369</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="n">
         <v>874</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+    <row r="59">
+      <c r="A59" s="2" t="n">
         <v>44588</v>
       </c>
-      <c r="B59">
+      <c r="B59" t="n">
         <v>375</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="n">
         <v>942</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+    <row r="60">
+      <c r="A60" s="2" t="n">
         <v>44589</v>
       </c>
-      <c r="B60">
+      <c r="B60" t="n">
         <v>407</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="n">
         <v>761</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+    <row r="61">
+      <c r="A61" s="2" t="n">
         <v>44590</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="n">
         <v>401</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="n">
         <v>1447</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+    <row r="62">
+      <c r="A62" s="2" t="n">
         <v>44591</v>
       </c>
-      <c r="B62">
+      <c r="B62" t="n">
         <v>424</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="n">
         <v>1188</v>
       </c>
-      <c r="D62">
+      <c r="D62" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+    <row r="63">
+      <c r="A63" s="2" t="n">
         <v>44592</v>
       </c>
-      <c r="B63">
+      <c r="B63" t="n">
         <v>443</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="n">
         <v>1259</v>
       </c>
-      <c r="D63">
+      <c r="D63" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+    <row r="64">
+      <c r="A64" s="2" t="n">
         <v>44593</v>
       </c>
-      <c r="B64">
+      <c r="B64" t="n">
         <v>460</v>
       </c>
-      <c r="C64">
+      <c r="C64" t="n">
         <v>1043</v>
       </c>
-      <c r="D64">
+      <c r="D64" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+    <row r="65">
+      <c r="A65" s="2" t="n">
         <v>44594</v>
       </c>
-      <c r="B65">
+      <c r="B65" t="n">
         <v>444</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="n">
         <v>1146</v>
       </c>
-      <c r="D65">
+      <c r="D65" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+    <row r="66">
+      <c r="A66" s="2" t="n">
         <v>44595</v>
       </c>
-      <c r="B66">
+      <c r="B66" t="n">
         <v>453</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="n">
         <v>1084</v>
       </c>
-      <c r="D66">
+      <c r="D66" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+    <row r="67">
+      <c r="A67" s="2" t="n">
         <v>44596</v>
       </c>
-      <c r="B67">
+      <c r="B67" t="n">
         <v>483</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="n">
         <v>1059</v>
       </c>
-      <c r="D67">
+      <c r="D67" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+    <row r="68">
+      <c r="A68" s="2" t="n">
         <v>44597</v>
       </c>
-      <c r="B68">
+      <c r="B68" t="n">
         <v>389</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="n">
         <v>1413</v>
       </c>
-      <c r="D68">
+      <c r="D68" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+    <row r="69">
+      <c r="A69" s="2" t="n">
         <v>44598</v>
       </c>
-      <c r="B69">
+      <c r="B69" t="n">
         <v>404</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="n">
         <v>1361</v>
       </c>
-      <c r="D69">
+      <c r="D69" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+    <row r="70">
+      <c r="A70" s="2" t="n">
         <v>44599</v>
       </c>
-      <c r="B70">
+      <c r="B70" t="n">
         <v>464</v>
       </c>
-      <c r="C70">
+      <c r="C70" t="n">
         <v>1276</v>
       </c>
-      <c r="D70">
+      <c r="D70" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+    <row r="71">
+      <c r="A71" s="2" t="n">
         <v>44600</v>
       </c>
-      <c r="B71">
+      <c r="B71" t="n">
         <v>438</v>
       </c>
-      <c r="C71">
+      <c r="C71" t="n">
         <v>1409</v>
       </c>
-      <c r="D71">
+      <c r="D71" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+    <row r="72">
+      <c r="A72" s="2" t="n">
         <v>44601</v>
       </c>
-      <c r="B72">
+      <c r="B72" t="n">
         <v>442</v>
       </c>
-      <c r="C72">
+      <c r="C72" t="n">
         <v>1501</v>
       </c>
-      <c r="D72">
+      <c r="D72" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+    <row r="73">
+      <c r="A73" s="2" t="n">
         <v>44602</v>
       </c>
-      <c r="B73">
+      <c r="B73" t="n">
         <v>459</v>
       </c>
-      <c r="C73">
+      <c r="C73" t="n">
         <v>1744</v>
       </c>
-      <c r="D73">
+      <c r="D73" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+    <row r="74">
+      <c r="A74" s="2" t="n">
         <v>44603</v>
       </c>
-      <c r="B74">
+      <c r="B74" t="n">
         <v>463</v>
       </c>
-      <c r="C74">
+      <c r="C74" t="n">
         <v>1922</v>
       </c>
-      <c r="D74">
+      <c r="D74" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+    <row r="75">
+      <c r="A75" s="2" t="n">
         <v>44604</v>
       </c>
-      <c r="B75">
+      <c r="B75" t="n">
         <v>521</v>
       </c>
-      <c r="C75">
+      <c r="C75" t="n">
         <v>1646</v>
       </c>
-      <c r="D75">
+      <c r="D75" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+    <row r="76">
+      <c r="A76" s="2" t="n">
         <v>44605</v>
       </c>
-      <c r="B76">
+      <c r="B76" t="n">
         <v>513</v>
       </c>
-      <c r="C76">
+      <c r="C76" t="n">
         <v>2013</v>
       </c>
-      <c r="D76">
+      <c r="D76" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+    <row r="77">
+      <c r="A77" s="2" t="n">
         <v>44606</v>
       </c>
-      <c r="B77">
+      <c r="B77" t="n">
         <v>510</v>
       </c>
-      <c r="C77">
+      <c r="C77" t="n">
         <v>2707</v>
       </c>
-      <c r="D77">
+      <c r="D77" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+    <row r="78">
+      <c r="A78" s="2" t="n">
         <v>44607</v>
       </c>
-      <c r="B78">
+      <c r="B78" t="n">
         <v>502</v>
       </c>
-      <c r="C78">
+      <c r="C78" t="n">
         <v>2454</v>
       </c>
-      <c r="D78">
+      <c r="D78" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+    <row r="79">
+      <c r="A79" s="2" t="n">
         <v>44608</v>
       </c>
-      <c r="B79">
+      <c r="B79" t="n">
         <v>525</v>
       </c>
-      <c r="C79">
+      <c r="C79" t="n">
         <v>2019</v>
       </c>
-      <c r="D79">
+      <c r="D79" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+    <row r="80">
+      <c r="A80" s="2" t="n">
         <v>44609</v>
       </c>
-      <c r="B80">
+      <c r="B80" t="n">
         <v>505</v>
       </c>
-      <c r="C80">
+      <c r="C80" t="n">
         <v>2351</v>
       </c>
-      <c r="D80">
+      <c r="D80" t="n">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+    <row r="81">
+      <c r="A81" s="2" t="n">
         <v>44610</v>
       </c>
-      <c r="B81">
+      <c r="B81" t="n">
         <v>558</v>
       </c>
-      <c r="C81">
+      <c r="C81" t="n">
         <v>1871</v>
       </c>
-      <c r="D81">
+      <c r="D81" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+    <row r="82">
+      <c r="A82" s="2" t="n">
         <v>44611</v>
       </c>
-      <c r="B82">
+      <c r="B82" t="n">
         <v>614</v>
       </c>
-      <c r="C82">
+      <c r="C82" t="n">
         <v>1462</v>
       </c>
-      <c r="D82">
+      <c r="D82" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+    <row r="83">
+      <c r="A83" s="2" t="n">
         <v>44612</v>
       </c>
-      <c r="B83">
+      <c r="B83" t="n">
         <v>603</v>
       </c>
-      <c r="C83">
+      <c r="C83" t="n">
         <v>1097</v>
       </c>
-      <c r="D83">
+      <c r="D83" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+    <row r="84">
+      <c r="A84" s="2" t="n">
         <v>44613</v>
       </c>
-      <c r="B84">
+      <c r="B84" t="n">
         <v>726</v>
       </c>
-      <c r="C84">
+      <c r="C84" t="n">
         <v>1071</v>
       </c>
-      <c r="D84">
+      <c r="D84" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+    <row r="85">
+      <c r="A85" s="2" t="n">
         <v>44614</v>
       </c>
-      <c r="B85">
+      <c r="B85" t="n">
         <v>607</v>
       </c>
-      <c r="C85">
+      <c r="C85" t="n">
         <v>1046</v>
       </c>
-      <c r="D85">
+      <c r="D85" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+    <row r="86">
+      <c r="A86" s="2" t="n">
         <v>44615</v>
       </c>
-      <c r="B86">
+      <c r="B86" t="n">
         <v>518</v>
       </c>
-      <c r="C86">
+      <c r="C86" t="n">
         <v>944</v>
       </c>
-      <c r="D86">
+      <c r="D86" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+    <row r="87">
+      <c r="A87" s="2" t="n">
         <v>44616</v>
       </c>
-      <c r="B87">
+      <c r="B87" t="n">
         <v>599</v>
       </c>
-      <c r="C87">
+      <c r="C87" t="n">
         <v>1136</v>
       </c>
-      <c r="D87">
+      <c r="D87" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+    <row r="88">
+      <c r="A88" s="2" t="n">
         <v>44617</v>
       </c>
-      <c r="B88">
+      <c r="B88" t="n">
         <v>531</v>
       </c>
-      <c r="C88">
+      <c r="C88" t="n">
         <v>1432</v>
       </c>
-      <c r="D88">
+      <c r="D88" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+    <row r="89">
+      <c r="A89" s="2" t="n">
         <v>44618</v>
       </c>
-      <c r="B89">
+      <c r="B89" t="n">
         <v>598</v>
       </c>
-      <c r="C89">
+      <c r="C89" t="n">
         <v>1388</v>
       </c>
-      <c r="D89">
+      <c r="D89" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+    <row r="90">
+      <c r="A90" s="2" t="n">
         <v>44619</v>
       </c>
-      <c r="B90">
+      <c r="B90" t="n">
         <v>516</v>
       </c>
-      <c r="C90">
+      <c r="C90" t="n">
         <v>1175</v>
       </c>
-      <c r="D90">
+      <c r="D90" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+    <row r="91">
+      <c r="A91" s="2" t="n">
         <v>44620</v>
       </c>
-      <c r="B91">
+      <c r="B91" t="n">
         <v>527</v>
       </c>
-      <c r="C91">
+      <c r="C91" t="n">
         <v>1272</v>
       </c>
-      <c r="D91">
+      <c r="D91" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+    <row r="92">
+      <c r="A92" s="2" t="n">
         <v>44621</v>
       </c>
-      <c r="B92">
+      <c r="B92" t="n">
         <v>505</v>
       </c>
-      <c r="C92">
+      <c r="C92" t="n">
         <v>1706</v>
       </c>
-      <c r="D92">
+      <c r="D92" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+    <row r="93">
+      <c r="A93" s="2" t="n">
         <v>44622</v>
       </c>
-      <c r="B93">
+      <c r="B93" t="n">
         <v>510</v>
       </c>
-      <c r="C93">
+      <c r="C93" t="n">
         <v>1325</v>
       </c>
-      <c r="D93">
+      <c r="D93" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+    <row r="94">
+      <c r="A94" s="2" t="n">
         <v>44623</v>
       </c>
-      <c r="B94">
+      <c r="B94" t="n">
         <v>459</v>
       </c>
-      <c r="C94">
+      <c r="C94" t="n">
         <v>1435</v>
       </c>
-      <c r="D94">
+      <c r="D94" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+    <row r="95">
+      <c r="A95" s="2" t="n">
         <v>44624</v>
       </c>
-      <c r="B95">
+      <c r="B95" t="n">
         <v>528</v>
       </c>
-      <c r="C95">
+      <c r="C95" t="n">
         <v>1214</v>
       </c>
-      <c r="D95">
+      <c r="D95" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+    <row r="96">
+      <c r="A96" s="2" t="n">
         <v>44625</v>
       </c>
-      <c r="B96">
+      <c r="B96" t="n">
         <v>536</v>
       </c>
-      <c r="C96">
+      <c r="C96" t="n">
         <v>1147</v>
       </c>
-      <c r="D96">
+      <c r="D96" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+    <row r="97">
+      <c r="A97" s="2" t="n">
         <v>44626</v>
       </c>
-      <c r="B97">
+      <c r="B97" t="n">
         <v>548</v>
       </c>
-      <c r="C97">
+      <c r="C97" t="n">
         <v>1386</v>
       </c>
-      <c r="D97">
+      <c r="D97" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+    <row r="98">
+      <c r="A98" s="2" t="n">
         <v>44627</v>
       </c>
-      <c r="B98">
+      <c r="B98" t="n">
         <v>468</v>
       </c>
-      <c r="C98">
+      <c r="C98" t="n">
         <v>1571</v>
       </c>
-      <c r="D98">
+      <c r="D98" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+    <row r="99">
+      <c r="A99" s="2" t="n">
         <v>44628</v>
       </c>
-      <c r="B99">
+      <c r="B99" t="n">
         <v>495</v>
       </c>
-      <c r="C99">
+      <c r="C99" t="n">
         <v>1392</v>
       </c>
-      <c r="D99">
+      <c r="D99" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+    <row r="100">
+      <c r="A100" s="2" t="n">
         <v>44629</v>
       </c>
-      <c r="B100">
+      <c r="B100" t="n">
         <v>526</v>
       </c>
-      <c r="C100">
+      <c r="C100" t="n">
         <v>1179</v>
       </c>
-      <c r="D100">
+      <c r="D100" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+    <row r="101">
+      <c r="A101" s="2" t="n">
         <v>44630</v>
       </c>
-      <c r="B101">
+      <c r="B101" t="n">
         <v>475</v>
       </c>
-      <c r="C101">
+      <c r="C101" t="n">
         <v>1292</v>
       </c>
-      <c r="D101">
+      <c r="D101" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+    <row r="102">
+      <c r="A102" s="2" t="n">
         <v>44631</v>
       </c>
-      <c r="B102">
+      <c r="B102" t="n">
         <v>517</v>
       </c>
-      <c r="C102">
+      <c r="C102" t="n">
         <v>1278</v>
       </c>
-      <c r="D102">
+      <c r="D102" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+    <row r="103">
+      <c r="A103" s="2" t="n">
         <v>44632</v>
       </c>
-      <c r="B103">
+      <c r="B103" t="n">
         <v>507</v>
       </c>
-      <c r="C103">
+      <c r="C103" t="n">
         <v>1400</v>
       </c>
-      <c r="D103">
+      <c r="D103" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+    <row r="104">
+      <c r="A104" s="2" t="n">
         <v>44633</v>
       </c>
-      <c r="B104">
+      <c r="B104" t="n">
         <v>534</v>
       </c>
-      <c r="C104">
+      <c r="C104" t="n">
         <v>1371</v>
       </c>
-      <c r="D104">
+      <c r="D104" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+    <row r="105">
+      <c r="A105" s="2" t="n">
         <v>44634</v>
       </c>
-      <c r="B105">
+      <c r="B105" t="n">
         <v>552</v>
       </c>
-      <c r="C105">
+      <c r="C105" t="n">
         <v>1341</v>
       </c>
-      <c r="D105">
+      <c r="D105" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+    <row r="106">
+      <c r="A106" s="2" t="n">
         <v>44635</v>
       </c>
-      <c r="B106">
+      <c r="B106" t="n">
         <v>514</v>
       </c>
-      <c r="C106">
+      <c r="C106" t="n">
         <v>1223</v>
       </c>
-      <c r="D106">
+      <c r="D106" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+    <row r="107">
+      <c r="A107" s="2" t="n">
         <v>44636</v>
       </c>
-      <c r="B107">
+      <c r="B107" t="n">
         <v>471</v>
       </c>
-      <c r="C107">
+      <c r="C107" t="n">
         <v>1439</v>
       </c>
-      <c r="D107">
+      <c r="D107" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+    <row r="108">
+      <c r="A108" s="2" t="n">
         <v>44637</v>
       </c>
-      <c r="B108">
+      <c r="B108" t="n">
         <v>472</v>
       </c>
-      <c r="C108">
+      <c r="C108" t="n">
         <v>1225</v>
       </c>
-      <c r="D108">
+      <c r="D108" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+    <row r="109">
+      <c r="A109" s="2" t="n">
         <v>44638</v>
       </c>
-      <c r="B109">
+      <c r="B109" t="n">
         <v>372</v>
       </c>
-      <c r="C109">
+      <c r="C109" t="n">
         <v>2442</v>
       </c>
-      <c r="D109">
+      <c r="D109" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+    <row r="110">
+      <c r="A110" s="2" t="n">
         <v>44639</v>
       </c>
-      <c r="B110">
+      <c r="B110" t="n">
         <v>480</v>
       </c>
-      <c r="C110">
+      <c r="C110" t="n">
         <v>2372</v>
       </c>
-      <c r="D110">
+      <c r="D110" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+    <row r="111">
+      <c r="A111" s="2" t="n">
         <v>44640</v>
       </c>
-      <c r="B111">
+      <c r="B111" t="n">
         <v>502</v>
       </c>
-      <c r="C111">
+      <c r="C111" t="n">
         <v>2572</v>
       </c>
-      <c r="D111">
+      <c r="D111" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+    <row r="112">
+      <c r="A112" s="2" t="n">
         <v>44641</v>
       </c>
-      <c r="B112">
+      <c r="B112" t="n">
         <v>532</v>
       </c>
-      <c r="C112">
+      <c r="C112" t="n">
         <v>2000</v>
       </c>
-      <c r="D112">
+      <c r="D112" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+    <row r="113">
+      <c r="A113" s="2" t="n">
         <v>44642</v>
       </c>
-      <c r="B113">
+      <c r="B113" t="n">
         <v>522</v>
       </c>
-      <c r="C113">
+      <c r="C113" t="n">
         <v>1336</v>
       </c>
-      <c r="D113">
+      <c r="D113" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+    <row r="114">
+      <c r="A114" s="2" t="n">
         <v>44643</v>
       </c>
-      <c r="B114">
+      <c r="B114" t="n">
         <v>483</v>
       </c>
-      <c r="C114">
+      <c r="C114" t="n">
         <v>1760</v>
       </c>
-      <c r="D114">
+      <c r="D114" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+    <row r="115">
+      <c r="A115" s="2" t="n">
         <v>44644</v>
       </c>
-      <c r="B115">
+      <c r="B115" t="n">
         <v>547</v>
       </c>
-      <c r="C115">
+      <c r="C115" t="n">
         <v>1321</v>
       </c>
-      <c r="D115">
+      <c r="D115" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+    <row r="116">
+      <c r="A116" s="2" t="n">
         <v>44645</v>
       </c>
-      <c r="B116">
+      <c r="B116" t="n">
         <v>470</v>
       </c>
-      <c r="C116">
+      <c r="C116" t="n">
         <v>1462</v>
       </c>
-      <c r="D116">
+      <c r="D116" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+    <row r="117">
+      <c r="A117" s="2" t="n">
         <v>44646</v>
       </c>
-      <c r="B117">
+      <c r="B117" t="n">
         <v>502</v>
       </c>
-      <c r="C117">
+      <c r="C117" t="n">
         <v>2136</v>
       </c>
-      <c r="D117">
+      <c r="D117" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+    <row r="118">
+      <c r="A118" s="2" t="n">
         <v>44647</v>
       </c>
-      <c r="B118">
+      <c r="B118" t="n">
         <v>497</v>
       </c>
-      <c r="C118">
+      <c r="C118" t="n">
         <v>2360</v>
       </c>
-      <c r="D118">
+      <c r="D118" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+    <row r="119">
+      <c r="A119" s="2" t="n">
         <v>44648</v>
       </c>
-      <c r="B119">
+      <c r="B119" t="n">
         <v>486</v>
       </c>
-      <c r="C119">
+      <c r="C119" t="n">
         <v>1640</v>
       </c>
-      <c r="D119">
+      <c r="D119" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+    <row r="120">
+      <c r="A120" s="2" t="n">
         <v>44649</v>
       </c>
-      <c r="B120">
+      <c r="B120" t="n">
         <v>514</v>
       </c>
-      <c r="C120">
+      <c r="C120" t="n">
         <v>2038</v>
       </c>
-      <c r="D120">
+      <c r="D120" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+    <row r="121">
+      <c r="A121" s="2" t="n">
         <v>44650</v>
       </c>
-      <c r="B121">
+      <c r="B121" t="n">
         <v>431</v>
       </c>
-      <c r="C121">
+      <c r="C121" t="n">
         <v>2479</v>
       </c>
-      <c r="D121">
+      <c r="D121" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+    <row r="122">
+      <c r="A122" s="2" t="n">
         <v>44651</v>
       </c>
-      <c r="B122">
+      <c r="B122" t="n">
         <v>464</v>
       </c>
-      <c r="C122">
+      <c r="C122" t="n">
         <v>1961</v>
       </c>
-      <c r="D122">
+      <c r="D122" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+    <row r="123">
+      <c r="A123" s="2" t="n">
         <v>44652</v>
       </c>
-      <c r="B123">
+      <c r="B123" t="n">
         <v>545</v>
       </c>
-      <c r="C123">
+      <c r="C123" t="n">
         <v>2326</v>
       </c>
-      <c r="D123">
+      <c r="D123" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+    <row r="124">
+      <c r="A124" s="2" t="n">
         <v>44653</v>
       </c>
-      <c r="B124">
+      <c r="B124" t="n">
         <v>527</v>
       </c>
-      <c r="C124">
+      <c r="C124" t="n">
         <v>2434</v>
       </c>
-      <c r="D124">
+      <c r="D124" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+    <row r="125">
+      <c r="A125" s="2" t="n">
         <v>44654</v>
       </c>
-      <c r="B125">
+      <c r="B125" t="n">
         <v>501</v>
       </c>
-      <c r="C125">
+      <c r="C125" t="n">
         <v>2208</v>
       </c>
-      <c r="D125">
+      <c r="D125" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+    <row r="126">
+      <c r="A126" s="2" t="n">
         <v>44655</v>
       </c>
-      <c r="B126">
+      <c r="B126" t="n">
         <v>498</v>
       </c>
-      <c r="C126">
+      <c r="C126" t="n">
         <v>2348</v>
       </c>
-      <c r="D126">
+      <c r="D126" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+    <row r="127">
+      <c r="A127" s="2" t="n">
         <v>44656</v>
       </c>
-      <c r="B127">
+      <c r="B127" t="n">
         <v>456</v>
       </c>
-      <c r="C127">
+      <c r="C127" t="n">
         <v>2252</v>
       </c>
-      <c r="D127">
+      <c r="D127" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+    <row r="128">
+      <c r="A128" s="2" t="n">
         <v>44657</v>
       </c>
-      <c r="B128">
+      <c r="B128" t="n">
         <v>485</v>
       </c>
-      <c r="C128">
+      <c r="C128" t="n">
         <v>2293</v>
       </c>
-      <c r="D128">
+      <c r="D128" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+    <row r="129">
+      <c r="A129" s="2" t="n">
         <v>44658</v>
       </c>
-      <c r="B129">
+      <c r="B129" t="n">
         <v>464</v>
       </c>
-      <c r="C129">
+      <c r="C129" t="n">
         <v>1965</v>
       </c>
-      <c r="D129">
+      <c r="D129" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+    <row r="130">
+      <c r="A130" s="2" t="n">
         <v>44659</v>
       </c>
-      <c r="B130">
+      <c r="B130" t="n">
         <v>521</v>
       </c>
-      <c r="C130">
+      <c r="C130" t="n">
         <v>1932</v>
       </c>
-      <c r="D130">
+      <c r="D130" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+    <row r="131">
+      <c r="A131" s="2" t="n">
         <v>44660</v>
       </c>
-      <c r="B131">
+      <c r="B131" t="n">
         <v>492</v>
       </c>
-      <c r="C131">
+      <c r="C131" t="n">
         <v>2235</v>
       </c>
-      <c r="D131">
+      <c r="D131" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+    <row r="132">
+      <c r="A132" s="2" t="n">
         <v>44661</v>
       </c>
-      <c r="B132">
+      <c r="B132" t="n">
         <v>593</v>
       </c>
-      <c r="C132">
+      <c r="C132" t="n">
         <v>2071</v>
       </c>
-      <c r="D132">
+      <c r="D132" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+    <row r="133">
+      <c r="A133" s="2" t="n">
         <v>44662</v>
       </c>
-      <c r="B133">
+      <c r="B133" t="n">
         <v>578</v>
       </c>
-      <c r="C133">
+      <c r="C133" t="n">
         <v>1735</v>
       </c>
-      <c r="D133">
+      <c r="D133" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+    <row r="134">
+      <c r="A134" s="2" t="n">
         <v>44663</v>
       </c>
-      <c r="B134">
+      <c r="B134" t="n">
         <v>506</v>
       </c>
-      <c r="C134">
+      <c r="C134" t="n">
         <v>1710</v>
       </c>
-      <c r="D134">
+      <c r="D134" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+    <row r="135">
+      <c r="A135" s="2" t="n">
         <v>44664</v>
       </c>
-      <c r="B135">
+      <c r="B135" t="n">
         <v>506</v>
       </c>
-      <c r="C135">
+      <c r="C135" t="n">
         <v>1778</v>
       </c>
-      <c r="D135">
+      <c r="D135" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+    <row r="136">
+      <c r="A136" s="2" t="n">
         <v>44665</v>
       </c>
-      <c r="B136">
+      <c r="B136" t="n">
         <v>544</v>
       </c>
-      <c r="C136">
+      <c r="C136" t="n">
         <v>1385</v>
       </c>
-      <c r="D136">
+      <c r="D136" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+    <row r="137">
+      <c r="A137" s="2" t="n">
         <v>44666</v>
       </c>
-      <c r="B137">
+      <c r="B137" t="n">
         <v>557</v>
       </c>
-      <c r="C137">
+      <c r="C137" t="n">
         <v>1466</v>
       </c>
-      <c r="D137">
+      <c r="D137" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+    <row r="138">
+      <c r="A138" s="2" t="n">
         <v>44667</v>
       </c>
-      <c r="B138">
+      <c r="B138" t="n">
         <v>346</v>
       </c>
-      <c r="C138">
+      <c r="C138" t="n">
         <v>1568</v>
       </c>
-      <c r="D138">
+      <c r="D138" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+    <row r="139">
+      <c r="A139" s="2" t="n">
         <v>44668</v>
       </c>
-      <c r="B139">
+      <c r="B139" t="n">
         <v>573</v>
       </c>
-      <c r="C139">
+      <c r="C139" t="n">
         <v>2004</v>
       </c>
-      <c r="D139">
+      <c r="D139" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+    <row r="140">
+      <c r="A140" s="2" t="n">
         <v>44669</v>
       </c>
-      <c r="B140">
+      <c r="B140" t="n">
         <v>538</v>
       </c>
-      <c r="C140">
+      <c r="C140" t="n">
         <v>1875</v>
       </c>
-      <c r="D140">
+      <c r="D140" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+    <row r="141">
+      <c r="A141" s="2" t="n">
         <v>44670</v>
       </c>
-      <c r="B141">
+      <c r="B141" t="n">
         <v>547</v>
       </c>
-      <c r="C141">
+      <c r="C141" t="n">
         <v>1836</v>
       </c>
-      <c r="D141">
+      <c r="D141" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+    <row r="142">
+      <c r="A142" s="2" t="n">
         <v>44671</v>
       </c>
-      <c r="B142">
+      <c r="B142" t="n">
         <v>567</v>
       </c>
-      <c r="C142">
+      <c r="C142" t="n">
         <v>1223</v>
       </c>
-      <c r="D142">
+      <c r="D142" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+    <row r="143">
+      <c r="A143" s="2" t="n">
         <v>44672</v>
       </c>
-      <c r="B143">
+      <c r="B143" t="n">
         <v>556</v>
       </c>
-      <c r="C143">
+      <c r="C143" t="n">
         <v>1215</v>
       </c>
-      <c r="D143">
+      <c r="D143" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+    <row r="144">
+      <c r="A144" s="2" t="n">
         <v>44673</v>
       </c>
-      <c r="B144">
+      <c r="B144" t="n">
         <v>470</v>
       </c>
-      <c r="C144">
+      <c r="C144" t="n">
         <v>1163</v>
       </c>
-      <c r="D144">
+      <c r="D144" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+    <row r="145">
+      <c r="A145" s="2" t="n">
         <v>44674</v>
       </c>
-      <c r="B145">
+      <c r="B145" t="n">
         <v>446</v>
       </c>
-      <c r="C145">
+      <c r="C145" t="n">
         <v>1886</v>
       </c>
-      <c r="D145">
+      <c r="D145" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+    <row r="146">
+      <c r="A146" s="2" t="n">
         <v>44675</v>
       </c>
-      <c r="B146">
+      <c r="B146" t="n">
         <v>518</v>
       </c>
-      <c r="C146">
+      <c r="C146" t="n">
         <v>1916</v>
       </c>
-      <c r="D146">
+      <c r="D146" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+    <row r="147">
+      <c r="A147" s="2" t="n">
         <v>44676</v>
       </c>
-      <c r="B147">
+      <c r="B147" t="n">
         <v>305</v>
       </c>
-      <c r="C147">
+      <c r="C147" t="n">
         <v>1513</v>
       </c>
-      <c r="D147">
+      <c r="D147" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+    <row r="148">
+      <c r="A148" s="2" t="n">
         <v>44677</v>
       </c>
-      <c r="B148">
+      <c r="B148" t="n">
         <v>115</v>
       </c>
-      <c r="C148">
+      <c r="C148" t="n">
         <v>1130</v>
       </c>
-      <c r="D148">
+      <c r="D148" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+    <row r="149">
+      <c r="A149" s="2" t="n">
         <v>44678</v>
       </c>
-      <c r="B149">
+      <c r="B149" t="n">
         <v>154</v>
       </c>
-      <c r="C149">
+      <c r="C149" t="n">
         <v>1430</v>
       </c>
-      <c r="D149">
+      <c r="D149" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+    <row r="150">
+      <c r="A150" s="2" t="n">
         <v>44679</v>
       </c>
-      <c r="B150">
+      <c r="B150" t="n">
         <v>159</v>
       </c>
-      <c r="C150">
+      <c r="C150" t="n">
         <v>1243</v>
       </c>
-      <c r="D150">
+      <c r="D150" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+    <row r="151">
+      <c r="A151" s="2" t="n">
         <v>44680</v>
       </c>
-      <c r="B151">
+      <c r="B151" t="n">
         <v>131</v>
       </c>
-      <c r="C151">
+      <c r="C151" t="n">
         <v>1323</v>
       </c>
-      <c r="D151">
+      <c r="D151" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+    <row r="152">
+      <c r="A152" s="2" t="n">
         <v>44681</v>
       </c>
-      <c r="B152">
+      <c r="B152" t="n">
         <v>282</v>
       </c>
-      <c r="C152">
+      <c r="C152" t="n">
         <v>1394</v>
       </c>
-      <c r="D152">
+      <c r="D152" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+    <row r="153">
+      <c r="A153" s="2" t="n">
         <v>44682</v>
       </c>
-      <c r="B153">
+      <c r="B153" t="n">
         <v>274</v>
       </c>
-      <c r="C153">
+      <c r="C153" t="n">
         <v>1834</v>
       </c>
-      <c r="D153">
+      <c r="D153" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+    <row r="154">
+      <c r="A154" s="2" t="n">
         <v>44683</v>
       </c>
-      <c r="B154">
+      <c r="B154" t="n">
         <v>154</v>
       </c>
-      <c r="C154">
+      <c r="C154" t="n">
         <v>1906</v>
       </c>
-      <c r="D154">
+      <c r="D154" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+    <row r="155">
+      <c r="A155" s="2" t="n">
         <v>44684</v>
       </c>
-      <c r="B155">
+      <c r="B155" t="n">
         <v>133</v>
       </c>
-      <c r="C155">
+      <c r="C155" t="n">
         <v>1743</v>
       </c>
-      <c r="D155">
+      <c r="D155" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+    <row r="156">
+      <c r="A156" s="2" t="n">
         <v>44685</v>
       </c>
-      <c r="B156">
+      <c r="B156" t="n">
         <v>122</v>
       </c>
-      <c r="C156">
+      <c r="C156" t="n">
         <v>1566</v>
       </c>
-      <c r="D156">
+      <c r="D156" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+    <row r="157">
+      <c r="A157" s="2" t="n">
         <v>44686</v>
       </c>
-      <c r="B157">
+      <c r="B157" t="n">
         <v>238</v>
       </c>
-      <c r="C157">
+      <c r="C157" t="n">
         <v>1197</v>
       </c>
-      <c r="D157">
+      <c r="D157" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+    <row r="158">
+      <c r="A158" s="2" t="n">
         <v>44687</v>
       </c>
-      <c r="B158">
+      <c r="B158" t="n">
         <v>106</v>
       </c>
-      <c r="C158">
+      <c r="C158" t="n">
         <v>1624</v>
       </c>
-      <c r="D158">
+      <c r="D158" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+    <row r="159">
+      <c r="A159" s="2" t="n">
         <v>44688</v>
       </c>
-      <c r="B159">
+      <c r="B159" t="n">
         <v>78</v>
       </c>
-      <c r="C159">
+      <c r="C159" t="n">
         <v>1822</v>
       </c>
-      <c r="D159">
+      <c r="D159" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+    <row r="160">
+      <c r="A160" s="2" t="n">
         <v>44689</v>
       </c>
-      <c r="B160">
+      <c r="B160" t="n">
         <v>215</v>
       </c>
-      <c r="C160">
+      <c r="C160" t="n">
         <v>1545</v>
       </c>
-      <c r="D160">
+      <c r="D160" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+    <row r="161">
+      <c r="A161" s="2" t="n">
         <v>44690</v>
       </c>
-      <c r="B161">
+      <c r="B161" t="n">
         <v>181</v>
       </c>
-      <c r="C161">
+      <c r="C161" t="n">
         <v>2050</v>
       </c>
-      <c r="D161">
+      <c r="D161" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+    <row r="162">
+      <c r="A162" s="2" t="n">
         <v>44691</v>
       </c>
-      <c r="B162">
+      <c r="B162" t="n">
         <v>166</v>
       </c>
-      <c r="C162">
+      <c r="C162" t="n">
         <v>1938</v>
       </c>
-      <c r="D162">
+      <c r="D162" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+    <row r="163">
+      <c r="A163" s="2" t="n">
         <v>44692</v>
       </c>
-      <c r="B163">
+      <c r="B163" t="n">
         <v>221</v>
       </c>
-      <c r="C163">
+      <c r="C163" t="n">
         <v>1382</v>
       </c>
-      <c r="D163">
+      <c r="D163" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+    <row r="164">
+      <c r="A164" s="2" t="n">
         <v>44693</v>
       </c>
-      <c r="B164">
+      <c r="B164" t="n">
         <v>238</v>
       </c>
-      <c r="C164">
+      <c r="C164" t="n">
         <v>1214</v>
       </c>
-      <c r="D164">
+      <c r="D164" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+    <row r="165">
+      <c r="A165" s="2" t="n">
         <v>44694</v>
       </c>
-      <c r="B165">
+      <c r="B165" t="n">
         <v>177</v>
       </c>
-      <c r="C165">
+      <c r="C165" t="n">
         <v>1816</v>
       </c>
-      <c r="D165">
+      <c r="D165" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+    <row r="166">
+      <c r="A166" s="2" t="n">
         <v>44695</v>
       </c>
-      <c r="B166">
+      <c r="B166" t="n">
         <v>260</v>
       </c>
-      <c r="C166">
+      <c r="C166" t="n">
         <v>1771</v>
       </c>
-      <c r="D166">
+      <c r="D166" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+    <row r="167">
+      <c r="A167" s="2" t="n">
         <v>44696</v>
       </c>
-      <c r="B167">
+      <c r="B167" t="n">
         <v>129</v>
       </c>
-      <c r="C167">
+      <c r="C167" t="n">
         <v>1584</v>
       </c>
-      <c r="D167">
+      <c r="D167" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+    <row r="168">
+      <c r="A168" s="2" t="n">
         <v>44697</v>
       </c>
-      <c r="B168">
+      <c r="B168" t="n">
         <v>156</v>
       </c>
-      <c r="C168">
+      <c r="C168" t="n">
         <v>1459</v>
       </c>
-      <c r="D168">
+      <c r="D168" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+    <row r="169">
+      <c r="A169" s="2" t="n">
         <v>44698</v>
       </c>
-      <c r="B169">
+      <c r="B169" t="n">
         <v>109</v>
       </c>
-      <c r="C169">
+      <c r="C169" t="n">
         <v>1232</v>
       </c>
-      <c r="D169">
+      <c r="D169" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+    <row r="170">
+      <c r="A170" s="2" t="n">
         <v>44699</v>
       </c>
-      <c r="B170">
+      <c r="B170" t="n">
         <v>107</v>
       </c>
-      <c r="C170">
+      <c r="C170" t="n">
         <v>1578</v>
       </c>
-      <c r="D170">
+      <c r="D170" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+    <row r="171">
+      <c r="A171" s="2" t="n">
         <v>44700</v>
       </c>
-      <c r="B171">
+      <c r="B171" t="n">
         <v>114</v>
       </c>
-      <c r="C171">
+      <c r="C171" t="n">
         <v>1266</v>
       </c>
-      <c r="D171">
+      <c r="D171" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+    <row r="172">
+      <c r="A172" s="2" t="n">
         <v>44701</v>
       </c>
-      <c r="B172">
+      <c r="B172" t="n">
         <v>113</v>
       </c>
-      <c r="C172">
+      <c r="C172" t="n">
         <v>1629</v>
       </c>
-      <c r="D172">
+      <c r="D172" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+    <row r="173">
+      <c r="A173" s="2" t="n">
         <v>44702</v>
       </c>
-      <c r="B173">
+      <c r="B173" t="n">
         <v>113</v>
       </c>
-      <c r="C173">
+      <c r="C173" t="n">
         <v>1279</v>
       </c>
-      <c r="D173">
+      <c r="D173" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+    <row r="174">
+      <c r="A174" s="2" t="n">
         <v>44703</v>
       </c>
-      <c r="B174">
+      <c r="B174" t="n">
         <v>117</v>
       </c>
-      <c r="C174">
+      <c r="C174" t="n">
         <v>1315</v>
       </c>
-      <c r="D174">
+      <c r="D174" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+    <row r="175">
+      <c r="A175" s="2" t="n">
         <v>44704</v>
       </c>
-      <c r="B175">
+      <c r="B175" t="n">
         <v>124</v>
       </c>
-      <c r="C175">
+      <c r="C175" t="n">
         <v>1813</v>
       </c>
-      <c r="D175">
+      <c r="D175" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+    <row r="176">
+      <c r="A176" s="2" t="n">
         <v>44705</v>
       </c>
-      <c r="B176">
+      <c r="B176" t="n">
         <v>139</v>
       </c>
-      <c r="C176">
+      <c r="C176" t="n">
         <v>1369</v>
       </c>
-      <c r="D176">
+      <c r="D176" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+    <row r="177">
+      <c r="A177" s="2" t="n">
         <v>44706</v>
       </c>
-      <c r="B177">
+      <c r="B177" t="n">
         <v>121</v>
       </c>
-      <c r="C177">
+      <c r="C177" t="n">
         <v>1182</v>
       </c>
-      <c r="D177">
+      <c r="D177" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+    <row r="178">
+      <c r="A178" s="2" t="n">
         <v>44707</v>
       </c>
-      <c r="B178">
+      <c r="B178" t="n">
         <v>124</v>
       </c>
-      <c r="C178">
+      <c r="C178" t="n">
         <v>969</v>
       </c>
-      <c r="D178">
+      <c r="D178" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+    <row r="179">
+      <c r="A179" s="2" t="n">
         <v>44708</v>
       </c>
-      <c r="B179">
+      <c r="B179" t="n">
         <v>109</v>
       </c>
-      <c r="C179">
+      <c r="C179" t="n">
         <v>1007</v>
       </c>
-      <c r="D179">
+      <c r="D179" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+    <row r="180">
+      <c r="A180" s="2" t="n">
         <v>44709</v>
       </c>
-      <c r="B180">
+      <c r="B180" t="n">
         <v>113</v>
       </c>
-      <c r="C180">
+      <c r="C180" t="n">
         <v>1336</v>
       </c>
-      <c r="D180">
+      <c r="D180" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+    <row r="181">
+      <c r="A181" s="2" t="n">
         <v>44710</v>
       </c>
-      <c r="B181">
+      <c r="B181" t="n">
         <v>120</v>
       </c>
-      <c r="C181">
+      <c r="C181" t="n">
         <v>1455</v>
       </c>
-      <c r="D181">
+      <c r="D181" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+    <row r="182">
+      <c r="A182" s="2" t="n">
         <v>44711</v>
       </c>
-      <c r="B182">
+      <c r="B182" t="n">
         <v>111</v>
       </c>
-      <c r="C182">
+      <c r="C182" t="n">
         <v>1653</v>
       </c>
-      <c r="D182">
+      <c r="D182" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+    <row r="183">
+      <c r="A183" s="2" t="n">
         <v>44712</v>
       </c>
-      <c r="B183">
+      <c r="B183" t="n">
         <v>84</v>
       </c>
-      <c r="C183">
+      <c r="C183" t="n">
         <v>1791</v>
       </c>
-      <c r="D183">
+      <c r="D183" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+    <row r="184">
+      <c r="A184" s="2" t="n">
         <v>44713</v>
       </c>
-      <c r="B184">
+      <c r="B184" t="n">
         <v>128</v>
       </c>
-      <c r="C184">
+      <c r="C184" t="n">
         <v>2083</v>
       </c>
-      <c r="D184">
+      <c r="D184" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+    <row r="185">
+      <c r="A185" s="2" t="n">
         <v>44714</v>
       </c>
-      <c r="B185">
+      <c r="B185" t="n">
         <v>121</v>
       </c>
-      <c r="C185">
+      <c r="C185" t="n">
         <v>1988</v>
       </c>
-      <c r="D185">
+      <c r="D185" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+    <row r="186">
+      <c r="A186" s="2" t="n">
         <v>44715</v>
       </c>
-      <c r="B186">
+      <c r="B186" t="n">
         <v>110</v>
       </c>
-      <c r="C186">
+      <c r="C186" t="n">
         <v>1586</v>
       </c>
-      <c r="D186">
+      <c r="D186" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+    <row r="187">
+      <c r="A187" s="2" t="n">
         <v>44716</v>
       </c>
-      <c r="B187">
+      <c r="B187" t="n">
         <v>115</v>
       </c>
-      <c r="C187">
+      <c r="C187" t="n">
         <v>1382</v>
       </c>
-      <c r="D187">
+      <c r="D187" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+    <row r="188">
+      <c r="A188" s="2" t="n">
         <v>44717</v>
       </c>
-      <c r="B188">
+      <c r="B188" t="n">
         <v>127</v>
       </c>
-      <c r="C188">
+      <c r="C188" t="n">
         <v>1294</v>
       </c>
-      <c r="D188">
+      <c r="D188" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+    <row r="189">
+      <c r="A189" s="2" t="n">
         <v>44718</v>
       </c>
-      <c r="B189">
+      <c r="B189" t="n">
         <v>124</v>
       </c>
-      <c r="C189">
+      <c r="C189" t="n">
         <v>1418</v>
       </c>
-      <c r="D189">
+      <c r="D189" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+    <row r="190">
+      <c r="A190" s="2" t="n">
         <v>44719</v>
       </c>
-      <c r="B190">
+      <c r="B190" t="n">
         <v>118</v>
       </c>
-      <c r="C190">
+      <c r="C190" t="n">
         <v>1592</v>
       </c>
-      <c r="D190">
+      <c r="D190" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+    <row r="191">
+      <c r="A191" s="2" t="n">
         <v>44720</v>
       </c>
-      <c r="B191">
+      <c r="B191" t="n">
         <v>120</v>
       </c>
-      <c r="C191">
+      <c r="C191" t="n">
         <v>1924</v>
       </c>
-      <c r="D191">
+      <c r="D191" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+    <row r="192">
+      <c r="A192" s="2" t="n">
         <v>44721</v>
       </c>
-      <c r="B192">
+      <c r="B192" t="n">
         <v>112</v>
       </c>
-      <c r="C192">
+      <c r="C192" t="n">
         <v>1910</v>
       </c>
-      <c r="D192">
+      <c r="D192" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+    <row r="193">
+      <c r="A193" s="2" t="n">
         <v>44722</v>
       </c>
-      <c r="B193">
+      <c r="B193" t="n">
         <v>114</v>
       </c>
-      <c r="C193">
+      <c r="C193" t="n">
         <v>1850</v>
       </c>
-      <c r="D193">
+      <c r="D193" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+    <row r="194">
+      <c r="A194" s="2" t="n">
         <v>44723</v>
       </c>
-      <c r="B194">
+      <c r="B194" t="n">
         <v>115</v>
       </c>
-      <c r="C194">
+      <c r="C194" t="n">
         <v>2166</v>
       </c>
-      <c r="D194">
+      <c r="D194" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+    <row r="195">
+      <c r="A195" s="2" t="n">
         <v>44724</v>
       </c>
-      <c r="B195">
+      <c r="B195" t="n">
         <v>112</v>
       </c>
-      <c r="C195">
+      <c r="C195" t="n">
         <v>1680</v>
       </c>
-      <c r="D195">
+      <c r="D195" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+    <row r="196">
+      <c r="A196" s="2" t="n">
         <v>44725</v>
       </c>
-      <c r="B196">
+      <c r="B196" t="n">
         <v>117</v>
       </c>
-      <c r="C196">
+      <c r="C196" t="n">
         <v>1934</v>
       </c>
-      <c r="D196">
+      <c r="D196" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+    <row r="197">
+      <c r="A197" s="2" t="n">
         <v>44726</v>
       </c>
-      <c r="B197">
+      <c r="B197" t="n">
         <v>130</v>
       </c>
-      <c r="C197">
+      <c r="C197" t="n">
         <v>2094</v>
       </c>
-      <c r="D197">
+      <c r="D197" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+    <row r="198">
+      <c r="A198" s="2" t="n">
         <v>44727</v>
       </c>
-      <c r="B198">
+      <c r="B198" t="n">
         <v>127</v>
       </c>
-      <c r="C198">
+      <c r="C198" t="n">
         <v>2039</v>
       </c>
-      <c r="D198">
+      <c r="D198" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+    <row r="199">
+      <c r="A199" s="2" t="n">
         <v>44728</v>
       </c>
-      <c r="B199">
+      <c r="B199" t="n">
         <v>136</v>
       </c>
-      <c r="C199">
+      <c r="C199" t="n">
         <v>2118</v>
       </c>
-      <c r="D199">
+      <c r="D199" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+    <row r="200">
+      <c r="A200" s="2" t="n">
         <v>44729</v>
       </c>
-      <c r="B200">
+      <c r="B200" t="n">
         <v>118</v>
       </c>
-      <c r="C200">
+      <c r="C200" t="n">
         <v>2191</v>
       </c>
-      <c r="D200">
+      <c r="D200" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+    <row r="201">
+      <c r="A201" s="2" t="n">
         <v>44730</v>
       </c>
-      <c r="B201">
+      <c r="B201" t="n">
         <v>128</v>
       </c>
-      <c r="C201">
+      <c r="C201" t="n">
         <v>1628</v>
       </c>
-      <c r="D201">
+      <c r="D201" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+    <row r="202">
+      <c r="A202" s="2" t="n">
         <v>44731</v>
       </c>
-      <c r="B202">
+      <c r="B202" t="n">
         <v>132</v>
       </c>
-      <c r="C202">
+      <c r="C202" t="n">
         <v>2196</v>
       </c>
-      <c r="D202">
+      <c r="D202" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+    <row r="203">
+      <c r="A203" s="2" t="n">
         <v>44732</v>
       </c>
-      <c r="B203">
+      <c r="B203" t="n">
         <v>125</v>
       </c>
-      <c r="C203">
+      <c r="C203" t="n">
         <v>1887</v>
       </c>
-      <c r="D203">
+      <c r="D203" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+    <row r="204">
+      <c r="A204" s="2" t="n">
         <v>44733</v>
       </c>
-      <c r="B204">
+      <c r="B204" t="n">
         <v>129</v>
       </c>
-      <c r="C204">
+      <c r="C204" t="n">
         <v>1538</v>
       </c>
-      <c r="D204">
+      <c r="D204" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+    <row r="205">
+      <c r="A205" s="2" t="n">
         <v>44734</v>
       </c>
-      <c r="B205">
+      <c r="B205" t="n">
         <v>119</v>
       </c>
-      <c r="C205">
+      <c r="C205" t="n">
         <v>1170</v>
       </c>
-      <c r="D205">
+      <c r="D205" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+    <row r="206">
+      <c r="A206" s="2" t="n">
         <v>44735</v>
       </c>
-      <c r="B206">
+      <c r="B206" t="n">
         <v>135</v>
       </c>
-      <c r="C206">
+      <c r="C206" t="n">
         <v>1374</v>
       </c>
-      <c r="D206">
+      <c r="D206" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+    <row r="207">
+      <c r="A207" s="2" t="n">
         <v>44736</v>
       </c>
-      <c r="B207">
+      <c r="B207" t="n">
         <v>118</v>
       </c>
-      <c r="C207">
+      <c r="C207" t="n">
         <v>1147</v>
       </c>
-      <c r="D207">
+      <c r="D207" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+    <row r="208">
+      <c r="A208" s="2" t="n">
         <v>44737</v>
       </c>
-      <c r="B208">
+      <c r="B208" t="n">
         <v>120</v>
       </c>
-      <c r="C208">
+      <c r="C208" t="n">
         <v>865</v>
       </c>
-      <c r="D208">
+      <c r="D208" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+    <row r="209">
+      <c r="A209" s="2" t="n">
         <v>44738</v>
       </c>
-      <c r="B209">
+      <c r="B209" t="n">
         <v>114</v>
       </c>
-      <c r="C209">
+      <c r="C209" t="n">
         <v>1218</v>
       </c>
-      <c r="D209">
+      <c r="D209" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="2">
+    <row r="210">
+      <c r="A210" s="2" t="n">
         <v>44739</v>
       </c>
-      <c r="B210">
+      <c r="B210" t="n">
         <v>106</v>
       </c>
-      <c r="C210">
+      <c r="C210" t="n">
         <v>1311</v>
       </c>
-      <c r="D210">
+      <c r="D210" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="2">
+    <row r="211">
+      <c r="A211" s="2" t="n">
         <v>44740</v>
       </c>
-      <c r="B211">
+      <c r="B211" t="n">
         <v>109</v>
       </c>
-      <c r="C211">
+      <c r="C211" t="n">
         <v>885</v>
       </c>
-      <c r="D211">
+      <c r="D211" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="2">
+    <row r="212">
+      <c r="A212" s="2" t="n">
         <v>44741</v>
       </c>
-      <c r="B212">
+      <c r="B212" t="n">
         <v>60</v>
       </c>
-      <c r="C212">
+      <c r="C212" t="n">
         <v>1000</v>
       </c>
-      <c r="D212">
+      <c r="D212" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+    <row r="213">
+      <c r="A213" s="2" t="n">
         <v>44742</v>
       </c>
-      <c r="B213">
+      <c r="B213" t="n">
         <v>65</v>
       </c>
-      <c r="C213">
+      <c r="C213" t="n">
         <v>875</v>
       </c>
-      <c r="D213">
+      <c r="D213" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated master dataset and Step 4 notebook with model improvements and refinements
</commit_message>
<xml_diff>
--- a/datasets/master_dataset/master_dataset.xlsx
+++ b/datasets/master_dataset/master_dataset.xlsx
@@ -1,40 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin\OneDrive\Documents\Infosys Springboard Internship Files\NitinMishra-Infosys-Nov24\datasets\master_dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5275F-4128-458F-A642-B11F5B62A0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Day Index</t>
+  </si>
+  <si>
+    <t>Clicks</t>
+  </si>
+  <si>
+    <t>Impressions</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,94 +72,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -424,3006 +397,2995 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Day Index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Clicks</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Impressions</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>44531</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>445</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>620</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>44532</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>433</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>890</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>44533</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>424</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>851</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>44534</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>427</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>881</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>44535</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>451</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>678</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>33</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>44536</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>429</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>995</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>44537</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>444</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>910</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>29</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>44538</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>431</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>867</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>24</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>44539</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>456</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>1128</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>23</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>44540</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>391</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1129</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>38</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>44541</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>447</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>1461</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>20</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>44542</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>347</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>1237</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>21</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>44543</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>443</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>1403</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>18</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>44544</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>427</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>1641</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>15</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>44545</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>423</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>1496</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>44546</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>404</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>1775</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>11</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>44547</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>413</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>1619</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>17</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>44548</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>370</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>969</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>14</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>44549</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>429</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>678</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>11</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>44550</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>383</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>1330</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>18</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>44551</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>379</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>1331</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>13</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>44552</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>350</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>1176</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>6</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>44553</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>359</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>1257</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>9</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>44554</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>339</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>1085</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>8</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>44555</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>338</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>1814</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>12</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>44556</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>398</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>1759</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>7</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>44557</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>369</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>1119</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>11</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>44558</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>381</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>893</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>13</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>44559</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>361</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>1028</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>12</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>44560</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>356</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>956</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>11</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>44561</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>237</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>911</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>15</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>44562</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>332</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>1350</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>12</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>44563</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>389</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>1704</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>26</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>44564</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>411</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>2177</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>28</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>44565</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>401</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>2549</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>14</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>44566</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>361</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>1915</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>23</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>44567</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>385</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>2125</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>18</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>44568</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>397</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>1984</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>23</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>44569</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>398</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>1859</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>16</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>44570</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>401</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>1759</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>19</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>44571</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>392</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>1571</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>18</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>44572</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>398</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>1818</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>18</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>44573</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>376</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>1506</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>21</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>44574</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>369</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>1724</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>15</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>44575</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>387</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>2196</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>16</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>44576</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>399</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>1933</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>11</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>44577</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>413</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>1959</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>16</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>44578</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>425</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>1689</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>19</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>44579</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>368</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>1524</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>16</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>44580</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>390</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>1041</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>16</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>44581</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>431</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>1175</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>18</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>44582</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>434</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>1681</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53">
         <v>24</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>44583</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>385</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>963</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>13</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>44584</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>444</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55">
         <v>783</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>14</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>44585</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>425</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>1040</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>26</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>44586</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>384</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>968</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57">
         <v>12</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>44587</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>369</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>874</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58">
         <v>18</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>44588</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>375</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>942</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>12</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>44589</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>407</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>761</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60">
         <v>13</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>44590</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>401</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61">
         <v>1447</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61">
         <v>14</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>44591</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>424</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>1188</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62">
         <v>9</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>44592</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>443</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63">
         <v>1259</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63">
         <v>15</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>44593</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>460</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64">
         <v>1043</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64">
         <v>25</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>44594</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>444</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>1146</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65">
         <v>13</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>44595</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>453</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66">
         <v>1084</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66">
         <v>21</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>44596</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>483</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67">
         <v>1059</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67">
         <v>23</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>44597</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>389</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>1413</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68">
         <v>15</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>44598</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>404</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69">
         <v>1361</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69">
         <v>12</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>44599</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>464</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70">
         <v>1276</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70">
         <v>22</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>44600</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>438</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>1409</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71">
         <v>17</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>44601</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>442</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>1501</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72">
         <v>20</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>44602</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>459</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73">
         <v>1744</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73">
         <v>23</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>44603</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>463</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74">
         <v>1922</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74">
         <v>16</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
         <v>44604</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>521</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75">
         <v>1646</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75">
         <v>15</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
         <v>44605</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>513</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76">
         <v>2013</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76">
         <v>27</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>44606</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>510</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77">
         <v>2707</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77">
         <v>19</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>44607</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>502</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>2454</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78">
         <v>17</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
         <v>44608</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>525</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>2019</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79">
         <v>22</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
         <v>44609</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>505</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80">
         <v>2351</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80">
         <v>38</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
         <v>44610</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>558</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81">
         <v>1871</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81">
         <v>28</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
         <v>44611</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>614</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82">
         <v>1462</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82">
         <v>23</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
         <v>44612</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>603</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83">
         <v>1097</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83">
         <v>15</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
         <v>44613</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>726</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>1071</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84">
         <v>26</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
         <v>44614</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>607</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85">
         <v>1046</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85">
         <v>18</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
         <v>44615</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>518</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86">
         <v>944</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86">
         <v>21</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
         <v>44616</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>599</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87">
         <v>1136</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87">
         <v>5</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
         <v>44617</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>531</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88">
         <v>1432</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88">
         <v>12</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
         <v>44618</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>598</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>1388</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89">
         <v>19</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
         <v>44619</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>516</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90">
         <v>1175</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90">
         <v>21</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
         <v>44620</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>527</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91">
         <v>1272</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91">
         <v>21</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
         <v>44621</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>505</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92">
         <v>1706</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92">
         <v>20</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
         <v>44622</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>510</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93">
         <v>1325</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93">
         <v>17</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
         <v>44623</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>459</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>1435</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94">
         <v>20</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
         <v>44624</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>528</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95">
         <v>1214</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95">
         <v>17</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
         <v>44625</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>536</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96">
         <v>1147</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96">
         <v>31</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
         <v>44626</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>548</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97">
         <v>1386</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97">
         <v>23</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
         <v>44627</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>468</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98">
         <v>1571</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98">
         <v>18</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
         <v>44628</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>495</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99">
         <v>1392</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99">
         <v>20</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
         <v>44629</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>526</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100">
         <v>1179</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100">
         <v>22</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
         <v>44630</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>475</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>1292</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101">
         <v>16</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
         <v>44631</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>517</v>
       </c>
-      <c r="C102" t="n">
+      <c r="C102">
         <v>1278</v>
       </c>
-      <c r="D102" t="n">
+      <c r="D102">
         <v>24</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
         <v>44632</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>507</v>
       </c>
-      <c r="C103" t="n">
+      <c r="C103">
         <v>1400</v>
       </c>
-      <c r="D103" t="n">
+      <c r="D103">
         <v>27</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
         <v>44633</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>534</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104">
         <v>1371</v>
       </c>
-      <c r="D104" t="n">
+      <c r="D104">
         <v>19</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
         <v>44634</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>552</v>
       </c>
-      <c r="C105" t="n">
+      <c r="C105">
         <v>1341</v>
       </c>
-      <c r="D105" t="n">
+      <c r="D105">
         <v>13</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
         <v>44635</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>514</v>
       </c>
-      <c r="C106" t="n">
+      <c r="C106">
         <v>1223</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D106">
         <v>15</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
         <v>44636</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>471</v>
       </c>
-      <c r="C107" t="n">
+      <c r="C107">
         <v>1439</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107">
         <v>17</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
         <v>44637</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>472</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>1225</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108">
         <v>15</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
         <v>44638</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>372</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109">
         <v>2442</v>
       </c>
-      <c r="D109" t="n">
+      <c r="D109">
         <v>19</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
         <v>44639</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>480</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>2372</v>
       </c>
-      <c r="D110" t="n">
+      <c r="D110">
         <v>25</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
         <v>44640</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>502</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C111">
         <v>2572</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111">
         <v>22</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
         <v>44641</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>532</v>
       </c>
-      <c r="C112" t="n">
+      <c r="C112">
         <v>2000</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112">
         <v>25</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
         <v>44642</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>522</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113">
         <v>1336</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D113">
         <v>7</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
         <v>44643</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>483</v>
       </c>
-      <c r="C114" t="n">
+      <c r="C114">
         <v>1760</v>
       </c>
-      <c r="D114" t="n">
+      <c r="D114">
         <v>15</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
         <v>44644</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>547</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115">
         <v>1321</v>
       </c>
-      <c r="D115" t="n">
+      <c r="D115">
         <v>32</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
         <v>44645</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>470</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116">
         <v>1462</v>
       </c>
-      <c r="D116" t="n">
+      <c r="D116">
         <v>24</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
         <v>44646</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>502</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117">
         <v>2136</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D117">
         <v>24</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
         <v>44647</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>497</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118">
         <v>2360</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D118">
         <v>21</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
         <v>44648</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>486</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>1640</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119">
         <v>21</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
         <v>44649</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>514</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120">
         <v>2038</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120">
         <v>18</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
         <v>44650</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>431</v>
       </c>
-      <c r="C121" t="n">
+      <c r="C121">
         <v>2479</v>
       </c>
-      <c r="D121" t="n">
+      <c r="D121">
         <v>19</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" s="2" t="n">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
         <v>44651</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B122">
         <v>464</v>
       </c>
-      <c r="C122" t="n">
+      <c r="C122">
         <v>1961</v>
       </c>
-      <c r="D122" t="n">
+      <c r="D122">
         <v>14</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="n">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
         <v>44652</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B123">
         <v>545</v>
       </c>
-      <c r="C123" t="n">
+      <c r="C123">
         <v>2326</v>
       </c>
-      <c r="D123" t="n">
+      <c r="D123">
         <v>9</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" s="2" t="n">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
         <v>44653</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B124">
         <v>527</v>
       </c>
-      <c r="C124" t="n">
+      <c r="C124">
         <v>2434</v>
       </c>
-      <c r="D124" t="n">
+      <c r="D124">
         <v>21</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" s="2" t="n">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
         <v>44654</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B125">
         <v>501</v>
       </c>
-      <c r="C125" t="n">
+      <c r="C125">
         <v>2208</v>
       </c>
-      <c r="D125" t="n">
+      <c r="D125">
         <v>24</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" s="2" t="n">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
         <v>44655</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B126">
         <v>498</v>
       </c>
-      <c r="C126" t="n">
+      <c r="C126">
         <v>2348</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126">
         <v>17</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="2" t="n">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
         <v>44656</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B127">
         <v>456</v>
       </c>
-      <c r="C127" t="n">
+      <c r="C127">
         <v>2252</v>
       </c>
-      <c r="D127" t="n">
+      <c r="D127">
         <v>21</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" s="2" t="n">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
         <v>44657</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B128">
         <v>485</v>
       </c>
-      <c r="C128" t="n">
+      <c r="C128">
         <v>2293</v>
       </c>
-      <c r="D128" t="n">
+      <c r="D128">
         <v>20</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" s="2" t="n">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
         <v>44658</v>
       </c>
-      <c r="B129" t="n">
+      <c r="B129">
         <v>464</v>
       </c>
-      <c r="C129" t="n">
+      <c r="C129">
         <v>1965</v>
       </c>
-      <c r="D129" t="n">
+      <c r="D129">
         <v>21</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="2" t="n">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
         <v>44659</v>
       </c>
-      <c r="B130" t="n">
+      <c r="B130">
         <v>521</v>
       </c>
-      <c r="C130" t="n">
+      <c r="C130">
         <v>1932</v>
       </c>
-      <c r="D130" t="n">
+      <c r="D130">
         <v>17</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="2" t="n">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
         <v>44660</v>
       </c>
-      <c r="B131" t="n">
+      <c r="B131">
         <v>492</v>
       </c>
-      <c r="C131" t="n">
+      <c r="C131">
         <v>2235</v>
       </c>
-      <c r="D131" t="n">
+      <c r="D131">
         <v>24</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="2" t="n">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
         <v>44661</v>
       </c>
-      <c r="B132" t="n">
+      <c r="B132">
         <v>593</v>
       </c>
-      <c r="C132" t="n">
+      <c r="C132">
         <v>2071</v>
       </c>
-      <c r="D132" t="n">
+      <c r="D132">
         <v>22</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" s="2" t="n">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
         <v>44662</v>
       </c>
-      <c r="B133" t="n">
+      <c r="B133">
         <v>578</v>
       </c>
-      <c r="C133" t="n">
+      <c r="C133">
         <v>1735</v>
       </c>
-      <c r="D133" t="n">
+      <c r="D133">
         <v>24</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" s="2" t="n">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
         <v>44663</v>
       </c>
-      <c r="B134" t="n">
+      <c r="B134">
         <v>506</v>
       </c>
-      <c r="C134" t="n">
+      <c r="C134">
         <v>1710</v>
       </c>
-      <c r="D134" t="n">
+      <c r="D134">
         <v>19</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" s="2" t="n">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
         <v>44664</v>
       </c>
-      <c r="B135" t="n">
+      <c r="B135">
         <v>506</v>
       </c>
-      <c r="C135" t="n">
+      <c r="C135">
         <v>1778</v>
       </c>
-      <c r="D135" t="n">
+      <c r="D135">
         <v>20</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" s="2" t="n">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
         <v>44665</v>
       </c>
-      <c r="B136" t="n">
+      <c r="B136">
         <v>544</v>
       </c>
-      <c r="C136" t="n">
+      <c r="C136">
         <v>1385</v>
       </c>
-      <c r="D136" t="n">
+      <c r="D136">
         <v>20</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="2" t="n">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
         <v>44666</v>
       </c>
-      <c r="B137" t="n">
+      <c r="B137">
         <v>557</v>
       </c>
-      <c r="C137" t="n">
+      <c r="C137">
         <v>1466</v>
       </c>
-      <c r="D137" t="n">
+      <c r="D137">
         <v>21</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" s="2" t="n">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
         <v>44667</v>
       </c>
-      <c r="B138" t="n">
+      <c r="B138">
         <v>346</v>
       </c>
-      <c r="C138" t="n">
+      <c r="C138">
         <v>1568</v>
       </c>
-      <c r="D138" t="n">
+      <c r="D138">
         <v>11</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="2" t="n">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
         <v>44668</v>
       </c>
-      <c r="B139" t="n">
+      <c r="B139">
         <v>573</v>
       </c>
-      <c r="C139" t="n">
+      <c r="C139">
         <v>2004</v>
       </c>
-      <c r="D139" t="n">
+      <c r="D139">
         <v>26</v>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" s="2" t="n">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
         <v>44669</v>
       </c>
-      <c r="B140" t="n">
+      <c r="B140">
         <v>538</v>
       </c>
-      <c r="C140" t="n">
+      <c r="C140">
         <v>1875</v>
       </c>
-      <c r="D140" t="n">
+      <c r="D140">
         <v>31</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" s="2" t="n">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
         <v>44670</v>
       </c>
-      <c r="B141" t="n">
+      <c r="B141">
         <v>547</v>
       </c>
-      <c r="C141" t="n">
+      <c r="C141">
         <v>1836</v>
       </c>
-      <c r="D141" t="n">
+      <c r="D141">
         <v>16</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" s="2" t="n">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
         <v>44671</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B142">
         <v>567</v>
       </c>
-      <c r="C142" t="n">
+      <c r="C142">
         <v>1223</v>
       </c>
-      <c r="D142" t="n">
+      <c r="D142">
         <v>16</v>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" s="2" t="n">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
         <v>44672</v>
       </c>
-      <c r="B143" t="n">
+      <c r="B143">
         <v>556</v>
       </c>
-      <c r="C143" t="n">
+      <c r="C143">
         <v>1215</v>
       </c>
-      <c r="D143" t="n">
+      <c r="D143">
         <v>30</v>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" s="2" t="n">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
         <v>44673</v>
       </c>
-      <c r="B144" t="n">
+      <c r="B144">
         <v>470</v>
       </c>
-      <c r="C144" t="n">
+      <c r="C144">
         <v>1163</v>
       </c>
-      <c r="D144" t="n">
+      <c r="D144">
         <v>36</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" s="2" t="n">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
         <v>44674</v>
       </c>
-      <c r="B145" t="n">
+      <c r="B145">
         <v>446</v>
       </c>
-      <c r="C145" t="n">
+      <c r="C145">
         <v>1886</v>
       </c>
-      <c r="D145" t="n">
+      <c r="D145">
         <v>16</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" s="2" t="n">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
         <v>44675</v>
       </c>
-      <c r="B146" t="n">
+      <c r="B146">
         <v>518</v>
       </c>
-      <c r="C146" t="n">
+      <c r="C146">
         <v>1916</v>
       </c>
-      <c r="D146" t="n">
+      <c r="D146">
         <v>17</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" s="2" t="n">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
         <v>44676</v>
       </c>
-      <c r="B147" t="n">
+      <c r="B147">
         <v>305</v>
       </c>
-      <c r="C147" t="n">
+      <c r="C147">
         <v>1513</v>
       </c>
-      <c r="D147" t="n">
+      <c r="D147">
         <v>23</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" s="2" t="n">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
         <v>44677</v>
       </c>
-      <c r="B148" t="n">
+      <c r="B148">
         <v>115</v>
       </c>
-      <c r="C148" t="n">
+      <c r="C148">
         <v>1130</v>
       </c>
-      <c r="D148" t="n">
+      <c r="D148">
         <v>17</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" s="2" t="n">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
         <v>44678</v>
       </c>
-      <c r="B149" t="n">
+      <c r="B149">
         <v>154</v>
       </c>
-      <c r="C149" t="n">
+      <c r="C149">
         <v>1430</v>
       </c>
-      <c r="D149" t="n">
+      <c r="D149">
         <v>14</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" s="2" t="n">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
         <v>44679</v>
       </c>
-      <c r="B150" t="n">
+      <c r="B150">
         <v>159</v>
       </c>
-      <c r="C150" t="n">
+      <c r="C150">
         <v>1243</v>
       </c>
-      <c r="D150" t="n">
+      <c r="D150">
         <v>12</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" s="2" t="n">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
         <v>44680</v>
       </c>
-      <c r="B151" t="n">
+      <c r="B151">
         <v>131</v>
       </c>
-      <c r="C151" t="n">
+      <c r="C151">
         <v>1323</v>
       </c>
-      <c r="D151" t="n">
+      <c r="D151">
         <v>11</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" s="2" t="n">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
         <v>44681</v>
       </c>
-      <c r="B152" t="n">
+      <c r="B152">
         <v>282</v>
       </c>
-      <c r="C152" t="n">
+      <c r="C152">
         <v>1394</v>
       </c>
-      <c r="D152" t="n">
+      <c r="D152">
         <v>23</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" s="2" t="n">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
         <v>44682</v>
       </c>
-      <c r="B153" t="n">
+      <c r="B153">
         <v>274</v>
       </c>
-      <c r="C153" t="n">
+      <c r="C153">
         <v>1834</v>
       </c>
-      <c r="D153" t="n">
+      <c r="D153">
         <v>9</v>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" s="2" t="n">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
         <v>44683</v>
       </c>
-      <c r="B154" t="n">
+      <c r="B154">
         <v>154</v>
       </c>
-      <c r="C154" t="n">
+      <c r="C154">
         <v>1906</v>
       </c>
-      <c r="D154" t="n">
+      <c r="D154">
         <v>19</v>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" s="2" t="n">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
         <v>44684</v>
       </c>
-      <c r="B155" t="n">
+      <c r="B155">
         <v>133</v>
       </c>
-      <c r="C155" t="n">
+      <c r="C155">
         <v>1743</v>
       </c>
-      <c r="D155" t="n">
+      <c r="D155">
         <v>25</v>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" s="2" t="n">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
         <v>44685</v>
       </c>
-      <c r="B156" t="n">
+      <c r="B156">
         <v>122</v>
       </c>
-      <c r="C156" t="n">
+      <c r="C156">
         <v>1566</v>
       </c>
-      <c r="D156" t="n">
+      <c r="D156">
         <v>16</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" s="2" t="n">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
         <v>44686</v>
       </c>
-      <c r="B157" t="n">
+      <c r="B157">
         <v>238</v>
       </c>
-      <c r="C157" t="n">
+      <c r="C157">
         <v>1197</v>
       </c>
-      <c r="D157" t="n">
+      <c r="D157">
         <v>18</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" s="2" t="n">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
         <v>44687</v>
       </c>
-      <c r="B158" t="n">
+      <c r="B158">
         <v>106</v>
       </c>
-      <c r="C158" t="n">
+      <c r="C158">
         <v>1624</v>
       </c>
-      <c r="D158" t="n">
+      <c r="D158">
         <v>14</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" s="2" t="n">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
         <v>44688</v>
       </c>
-      <c r="B159" t="n">
+      <c r="B159">
         <v>78</v>
       </c>
-      <c r="C159" t="n">
+      <c r="C159">
         <v>1822</v>
       </c>
-      <c r="D159" t="n">
+      <c r="D159">
         <v>21</v>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" s="2" t="n">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
         <v>44689</v>
       </c>
-      <c r="B160" t="n">
+      <c r="B160">
         <v>215</v>
       </c>
-      <c r="C160" t="n">
+      <c r="C160">
         <v>1545</v>
       </c>
-      <c r="D160" t="n">
+      <c r="D160">
         <v>14</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" s="2" t="n">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
         <v>44690</v>
       </c>
-      <c r="B161" t="n">
+      <c r="B161">
         <v>181</v>
       </c>
-      <c r="C161" t="n">
+      <c r="C161">
         <v>2050</v>
       </c>
-      <c r="D161" t="n">
+      <c r="D161">
         <v>15</v>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" s="2" t="n">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
         <v>44691</v>
       </c>
-      <c r="B162" t="n">
+      <c r="B162">
         <v>166</v>
       </c>
-      <c r="C162" t="n">
+      <c r="C162">
         <v>1938</v>
       </c>
-      <c r="D162" t="n">
+      <c r="D162">
         <v>13</v>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" s="2" t="n">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
         <v>44692</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B163">
         <v>221</v>
       </c>
-      <c r="C163" t="n">
+      <c r="C163">
         <v>1382</v>
       </c>
-      <c r="D163" t="n">
+      <c r="D163">
         <v>15</v>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" s="2" t="n">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
         <v>44693</v>
       </c>
-      <c r="B164" t="n">
+      <c r="B164">
         <v>238</v>
       </c>
-      <c r="C164" t="n">
+      <c r="C164">
         <v>1214</v>
       </c>
-      <c r="D164" t="n">
+      <c r="D164">
         <v>14</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" s="2" t="n">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
         <v>44694</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B165">
         <v>177</v>
       </c>
-      <c r="C165" t="n">
+      <c r="C165">
         <v>1816</v>
       </c>
-      <c r="D165" t="n">
+      <c r="D165">
         <v>11</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" s="2" t="n">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
         <v>44695</v>
       </c>
-      <c r="B166" t="n">
+      <c r="B166">
         <v>260</v>
       </c>
-      <c r="C166" t="n">
+      <c r="C166">
         <v>1771</v>
       </c>
-      <c r="D166" t="n">
+      <c r="D166">
         <v>19</v>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" s="2" t="n">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
         <v>44696</v>
       </c>
-      <c r="B167" t="n">
+      <c r="B167">
         <v>129</v>
       </c>
-      <c r="C167" t="n">
+      <c r="C167">
         <v>1584</v>
       </c>
-      <c r="D167" t="n">
+      <c r="D167">
         <v>12</v>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" s="2" t="n">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
         <v>44697</v>
       </c>
-      <c r="B168" t="n">
+      <c r="B168">
         <v>156</v>
       </c>
-      <c r="C168" t="n">
+      <c r="C168">
         <v>1459</v>
       </c>
-      <c r="D168" t="n">
+      <c r="D168">
         <v>12</v>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" s="2" t="n">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
         <v>44698</v>
       </c>
-      <c r="B169" t="n">
+      <c r="B169">
         <v>109</v>
       </c>
-      <c r="C169" t="n">
+      <c r="C169">
         <v>1232</v>
       </c>
-      <c r="D169" t="n">
+      <c r="D169">
         <v>11</v>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" s="2" t="n">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
         <v>44699</v>
       </c>
-      <c r="B170" t="n">
+      <c r="B170">
         <v>107</v>
       </c>
-      <c r="C170" t="n">
+      <c r="C170">
         <v>1578</v>
       </c>
-      <c r="D170" t="n">
+      <c r="D170">
         <v>11</v>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" s="2" t="n">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
         <v>44700</v>
       </c>
-      <c r="B171" t="n">
+      <c r="B171">
         <v>114</v>
       </c>
-      <c r="C171" t="n">
+      <c r="C171">
         <v>1266</v>
       </c>
-      <c r="D171" t="n">
+      <c r="D171">
         <v>20</v>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" s="2" t="n">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
         <v>44701</v>
       </c>
-      <c r="B172" t="n">
+      <c r="B172">
         <v>113</v>
       </c>
-      <c r="C172" t="n">
+      <c r="C172">
         <v>1629</v>
       </c>
-      <c r="D172" t="n">
+      <c r="D172">
         <v>13</v>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" s="2" t="n">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
         <v>44702</v>
       </c>
-      <c r="B173" t="n">
+      <c r="B173">
         <v>113</v>
       </c>
-      <c r="C173" t="n">
+      <c r="C173">
         <v>1279</v>
       </c>
-      <c r="D173" t="n">
+      <c r="D173">
         <v>10</v>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" s="2" t="n">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
         <v>44703</v>
       </c>
-      <c r="B174" t="n">
+      <c r="B174">
         <v>117</v>
       </c>
-      <c r="C174" t="n">
+      <c r="C174">
         <v>1315</v>
       </c>
-      <c r="D174" t="n">
+      <c r="D174">
         <v>20</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" s="2" t="n">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
         <v>44704</v>
       </c>
-      <c r="B175" t="n">
+      <c r="B175">
         <v>124</v>
       </c>
-      <c r="C175" t="n">
+      <c r="C175">
         <v>1813</v>
       </c>
-      <c r="D175" t="n">
+      <c r="D175">
         <v>14</v>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" s="2" t="n">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
         <v>44705</v>
       </c>
-      <c r="B176" t="n">
+      <c r="B176">
         <v>139</v>
       </c>
-      <c r="C176" t="n">
+      <c r="C176">
         <v>1369</v>
       </c>
-      <c r="D176" t="n">
+      <c r="D176">
         <v>19</v>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" s="2" t="n">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
         <v>44706</v>
       </c>
-      <c r="B177" t="n">
+      <c r="B177">
         <v>121</v>
       </c>
-      <c r="C177" t="n">
+      <c r="C177">
         <v>1182</v>
       </c>
-      <c r="D177" t="n">
+      <c r="D177">
         <v>10</v>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" s="2" t="n">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
         <v>44707</v>
       </c>
-      <c r="B178" t="n">
+      <c r="B178">
         <v>124</v>
       </c>
-      <c r="C178" t="n">
+      <c r="C178">
         <v>969</v>
       </c>
-      <c r="D178" t="n">
+      <c r="D178">
         <v>20</v>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" s="2" t="n">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
         <v>44708</v>
       </c>
-      <c r="B179" t="n">
+      <c r="B179">
         <v>109</v>
       </c>
-      <c r="C179" t="n">
+      <c r="C179">
         <v>1007</v>
       </c>
-      <c r="D179" t="n">
+      <c r="D179">
         <v>13</v>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" s="2" t="n">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
         <v>44709</v>
       </c>
-      <c r="B180" t="n">
+      <c r="B180">
         <v>113</v>
       </c>
-      <c r="C180" t="n">
+      <c r="C180">
         <v>1336</v>
       </c>
-      <c r="D180" t="n">
+      <c r="D180">
         <v>14</v>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" s="2" t="n">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
         <v>44710</v>
       </c>
-      <c r="B181" t="n">
+      <c r="B181">
         <v>120</v>
       </c>
-      <c r="C181" t="n">
+      <c r="C181">
         <v>1455</v>
       </c>
-      <c r="D181" t="n">
+      <c r="D181">
         <v>19</v>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" s="2" t="n">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
         <v>44711</v>
       </c>
-      <c r="B182" t="n">
+      <c r="B182">
         <v>111</v>
       </c>
-      <c r="C182" t="n">
+      <c r="C182">
         <v>1653</v>
       </c>
-      <c r="D182" t="n">
+      <c r="D182">
         <v>16</v>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
         <v>44712</v>
       </c>
-      <c r="B183" t="n">
+      <c r="B183">
         <v>84</v>
       </c>
-      <c r="C183" t="n">
+      <c r="C183">
         <v>1791</v>
       </c>
-      <c r="D183" t="n">
+      <c r="D183">
         <v>14</v>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" s="2" t="n">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
         <v>44713</v>
       </c>
-      <c r="B184" t="n">
+      <c r="B184">
         <v>128</v>
       </c>
-      <c r="C184" t="n">
+      <c r="C184">
         <v>2083</v>
       </c>
-      <c r="D184" t="n">
+      <c r="D184">
         <v>18</v>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" s="2" t="n">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
         <v>44714</v>
       </c>
-      <c r="B185" t="n">
+      <c r="B185">
         <v>121</v>
       </c>
-      <c r="C185" t="n">
+      <c r="C185">
         <v>1988</v>
       </c>
-      <c r="D185" t="n">
+      <c r="D185">
         <v>15</v>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" s="2" t="n">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
         <v>44715</v>
       </c>
-      <c r="B186" t="n">
+      <c r="B186">
         <v>110</v>
       </c>
-      <c r="C186" t="n">
+      <c r="C186">
         <v>1586</v>
       </c>
-      <c r="D186" t="n">
+      <c r="D186">
         <v>15</v>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" s="2" t="n">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
         <v>44716</v>
       </c>
-      <c r="B187" t="n">
+      <c r="B187">
         <v>115</v>
       </c>
-      <c r="C187" t="n">
+      <c r="C187">
         <v>1382</v>
       </c>
-      <c r="D187" t="n">
+      <c r="D187">
         <v>19</v>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" s="2" t="n">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
         <v>44717</v>
       </c>
-      <c r="B188" t="n">
+      <c r="B188">
         <v>127</v>
       </c>
-      <c r="C188" t="n">
+      <c r="C188">
         <v>1294</v>
       </c>
-      <c r="D188" t="n">
+      <c r="D188">
         <v>20</v>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" s="2" t="n">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
         <v>44718</v>
       </c>
-      <c r="B189" t="n">
+      <c r="B189">
         <v>124</v>
       </c>
-      <c r="C189" t="n">
+      <c r="C189">
         <v>1418</v>
       </c>
-      <c r="D189" t="n">
+      <c r="D189">
         <v>11</v>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" s="2" t="n">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
         <v>44719</v>
       </c>
-      <c r="B190" t="n">
+      <c r="B190">
         <v>118</v>
       </c>
-      <c r="C190" t="n">
+      <c r="C190">
         <v>1592</v>
       </c>
-      <c r="D190" t="n">
+      <c r="D190">
         <v>15</v>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" s="2" t="n">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
         <v>44720</v>
       </c>
-      <c r="B191" t="n">
+      <c r="B191">
         <v>120</v>
       </c>
-      <c r="C191" t="n">
+      <c r="C191">
         <v>1924</v>
       </c>
-      <c r="D191" t="n">
+      <c r="D191">
         <v>13</v>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" s="2" t="n">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
         <v>44721</v>
       </c>
-      <c r="B192" t="n">
+      <c r="B192">
         <v>112</v>
       </c>
-      <c r="C192" t="n">
+      <c r="C192">
         <v>1910</v>
       </c>
-      <c r="D192" t="n">
+      <c r="D192">
         <v>11</v>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" s="2" t="n">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
         <v>44722</v>
       </c>
-      <c r="B193" t="n">
+      <c r="B193">
         <v>114</v>
       </c>
-      <c r="C193" t="n">
+      <c r="C193">
         <v>1850</v>
       </c>
-      <c r="D193" t="n">
+      <c r="D193">
         <v>19</v>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" s="2" t="n">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
         <v>44723</v>
       </c>
-      <c r="B194" t="n">
+      <c r="B194">
         <v>115</v>
       </c>
-      <c r="C194" t="n">
+      <c r="C194">
         <v>2166</v>
       </c>
-      <c r="D194" t="n">
+      <c r="D194">
         <v>20</v>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" s="2" t="n">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
         <v>44724</v>
       </c>
-      <c r="B195" t="n">
+      <c r="B195">
         <v>112</v>
       </c>
-      <c r="C195" t="n">
+      <c r="C195">
         <v>1680</v>
       </c>
-      <c r="D195" t="n">
+      <c r="D195">
         <v>14</v>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" s="2" t="n">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
         <v>44725</v>
       </c>
-      <c r="B196" t="n">
+      <c r="B196">
         <v>117</v>
       </c>
-      <c r="C196" t="n">
+      <c r="C196">
         <v>1934</v>
       </c>
-      <c r="D196" t="n">
+      <c r="D196">
         <v>22</v>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" s="2" t="n">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
         <v>44726</v>
       </c>
-      <c r="B197" t="n">
+      <c r="B197">
         <v>130</v>
       </c>
-      <c r="C197" t="n">
+      <c r="C197">
         <v>2094</v>
       </c>
-      <c r="D197" t="n">
+      <c r="D197">
         <v>16</v>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" s="2" t="n">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
         <v>44727</v>
       </c>
-      <c r="B198" t="n">
+      <c r="B198">
         <v>127</v>
       </c>
-      <c r="C198" t="n">
+      <c r="C198">
         <v>2039</v>
       </c>
-      <c r="D198" t="n">
+      <c r="D198">
         <v>9</v>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" s="2" t="n">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
         <v>44728</v>
       </c>
-      <c r="B199" t="n">
+      <c r="B199">
         <v>136</v>
       </c>
-      <c r="C199" t="n">
+      <c r="C199">
         <v>2118</v>
       </c>
-      <c r="D199" t="n">
+      <c r="D199">
         <v>20</v>
       </c>
     </row>
-    <row r="200">
-      <c r="A200" s="2" t="n">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
         <v>44729</v>
       </c>
-      <c r="B200" t="n">
+      <c r="B200">
         <v>118</v>
       </c>
-      <c r="C200" t="n">
+      <c r="C200">
         <v>2191</v>
       </c>
-      <c r="D200" t="n">
+      <c r="D200">
         <v>15</v>
       </c>
     </row>
-    <row r="201">
-      <c r="A201" s="2" t="n">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
         <v>44730</v>
       </c>
-      <c r="B201" t="n">
+      <c r="B201">
         <v>128</v>
       </c>
-      <c r="C201" t="n">
+      <c r="C201">
         <v>1628</v>
       </c>
-      <c r="D201" t="n">
+      <c r="D201">
         <v>16</v>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" s="2" t="n">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
         <v>44731</v>
       </c>
-      <c r="B202" t="n">
+      <c r="B202">
         <v>132</v>
       </c>
-      <c r="C202" t="n">
+      <c r="C202">
         <v>2196</v>
       </c>
-      <c r="D202" t="n">
+      <c r="D202">
         <v>10</v>
       </c>
     </row>
-    <row r="203">
-      <c r="A203" s="2" t="n">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
         <v>44732</v>
       </c>
-      <c r="B203" t="n">
+      <c r="B203">
         <v>125</v>
       </c>
-      <c r="C203" t="n">
+      <c r="C203">
         <v>1887</v>
       </c>
-      <c r="D203" t="n">
+      <c r="D203">
         <v>15</v>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" s="2" t="n">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
         <v>44733</v>
       </c>
-      <c r="B204" t="n">
+      <c r="B204">
         <v>129</v>
       </c>
-      <c r="C204" t="n">
+      <c r="C204">
         <v>1538</v>
       </c>
-      <c r="D204" t="n">
+      <c r="D204">
         <v>7</v>
       </c>
     </row>
-    <row r="205">
-      <c r="A205" s="2" t="n">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
         <v>44734</v>
       </c>
-      <c r="B205" t="n">
+      <c r="B205">
         <v>119</v>
       </c>
-      <c r="C205" t="n">
+      <c r="C205">
         <v>1170</v>
       </c>
-      <c r="D205" t="n">
+      <c r="D205">
         <v>17</v>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" s="2" t="n">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
         <v>44735</v>
       </c>
-      <c r="B206" t="n">
+      <c r="B206">
         <v>135</v>
       </c>
-      <c r="C206" t="n">
+      <c r="C206">
         <v>1374</v>
       </c>
-      <c r="D206" t="n">
+      <c r="D206">
         <v>13</v>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" s="2" t="n">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
         <v>44736</v>
       </c>
-      <c r="B207" t="n">
+      <c r="B207">
         <v>118</v>
       </c>
-      <c r="C207" t="n">
+      <c r="C207">
         <v>1147</v>
       </c>
-      <c r="D207" t="n">
+      <c r="D207">
         <v>15</v>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" s="2" t="n">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
         <v>44737</v>
       </c>
-      <c r="B208" t="n">
+      <c r="B208">
         <v>120</v>
       </c>
-      <c r="C208" t="n">
+      <c r="C208">
         <v>865</v>
       </c>
-      <c r="D208" t="n">
+      <c r="D208">
         <v>16</v>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" s="2" t="n">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
         <v>44738</v>
       </c>
-      <c r="B209" t="n">
+      <c r="B209">
         <v>114</v>
       </c>
-      <c r="C209" t="n">
+      <c r="C209">
         <v>1218</v>
       </c>
-      <c r="D209" t="n">
+      <c r="D209">
         <v>13</v>
       </c>
     </row>
-    <row r="210">
-      <c r="A210" s="2" t="n">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
         <v>44739</v>
       </c>
-      <c r="B210" t="n">
+      <c r="B210">
         <v>106</v>
       </c>
-      <c r="C210" t="n">
+      <c r="C210">
         <v>1311</v>
       </c>
-      <c r="D210" t="n">
+      <c r="D210">
         <v>16</v>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" s="2" t="n">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
         <v>44740</v>
       </c>
-      <c r="B211" t="n">
+      <c r="B211">
         <v>109</v>
       </c>
-      <c r="C211" t="n">
+      <c r="C211">
         <v>885</v>
       </c>
-      <c r="D211" t="n">
+      <c r="D211">
         <v>13</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" s="2" t="n">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
         <v>44741</v>
       </c>
-      <c r="B212" t="n">
+      <c r="B212">
         <v>60</v>
       </c>
-      <c r="C212" t="n">
+      <c r="C212">
         <v>1000</v>
       </c>
-      <c r="D212" t="n">
+      <c r="D212">
         <v>16</v>
       </c>
     </row>
-    <row r="213">
-      <c r="A213" s="2" t="n">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
         <v>44742</v>
       </c>
-      <c r="B213" t="n">
+      <c r="B213">
         <v>65</v>
       </c>
-      <c r="C213" t="n">
+      <c r="C213">
         <v>875</v>
       </c>
-      <c r="D213" t="n">
+      <c r="D213">
         <v>8</v>
       </c>
     </row>

</xml_diff>